<commit_message>
updated teams and leagues to match actual - removed "doubleup"
</commit_message>
<xml_diff>
--- a/data/TT/League-2020.xlsx
+++ b/data/TT/League-2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\DjangoLeagueScheduler\data\TT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466AB8C5-7AD4-4636-B3A6-69CD916C0AE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB44E22-2771-4BEF-83B4-99AE3DA058EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26004" yWindow="2964" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablib Dataset" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,7 +484,7 @@
         <v>16</v>
       </c>
       <c r="F2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <v>120</v>
@@ -507,7 +507,7 @@
         <v>16</v>
       </c>
       <c r="F3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>120</v>
@@ -530,7 +530,7 @@
         <v>16</v>
       </c>
       <c r="F4">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G4">
         <v>105</v>
@@ -553,7 +553,7 @@
         <v>6</v>
       </c>
       <c r="F5">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G5">
         <v>105</v>

</xml_diff>

<commit_message>
tuned algorithm / added templates and generators1
</commit_message>
<xml_diff>
--- a/data/TT/League-2020.xlsx
+++ b/data/TT/League-2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\DjangoLeagueScheduler\data\TT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB44E22-2771-4BEF-83B4-99AE3DA058EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0379648-74A4-4F89-8392-FA1C59F0EA7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablib Dataset" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -439,7 +441,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,13 +486,13 @@
         <v>16</v>
       </c>
       <c r="F2">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G2">
         <v>120</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -507,13 +509,13 @@
         <v>16</v>
       </c>
       <c r="F3">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G3">
         <v>120</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -530,13 +532,13 @@
         <v>16</v>
       </c>
       <c r="F4">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="G4">
         <v>105</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -553,13 +555,13 @@
         <v>6</v>
       </c>
       <c r="F5">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="G5">
         <v>105</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -576,13 +578,13 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="G6">
         <v>90</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -599,13 +601,13 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="G7">
         <v>60</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -622,13 +624,13 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="G8">
         <v>60</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>